<commit_message>
Data exploration in project 5.
</commit_message>
<xml_diff>
--- a/5_IdentifyFraudFromEnronEmail/final_project/data_description.xlsx
+++ b/5_IdentifyFraudFromEnronEmail/final_project/data_description.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="25">
   <si>
     <t>count</t>
   </si>
@@ -1066,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,48 +1117,6 @@
       <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1177,48 +1135,6 @@
         <v>145</v>
       </c>
       <c r="F2" s="1">
-        <v>145</v>
-      </c>
-      <c r="G2" s="1">
-        <v>145</v>
-      </c>
-      <c r="H2" s="1">
-        <v>145</v>
-      </c>
-      <c r="I2">
-        <v>145</v>
-      </c>
-      <c r="J2" s="1">
-        <v>145</v>
-      </c>
-      <c r="K2" s="1">
-        <v>145</v>
-      </c>
-      <c r="L2" s="1">
-        <v>145</v>
-      </c>
-      <c r="M2" s="1">
-        <v>145</v>
-      </c>
-      <c r="N2">
-        <v>145</v>
-      </c>
-      <c r="O2" s="1">
-        <v>145</v>
-      </c>
-      <c r="P2">
-        <v>145</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>145</v>
-      </c>
-      <c r="R2" s="1">
-        <v>145</v>
-      </c>
-      <c r="S2" s="1">
-        <v>145</v>
-      </c>
-      <c r="T2">
         <v>145</v>
       </c>
       <c r="U2" s="1"/>
@@ -1244,48 +1160,6 @@
       <c r="F3" s="1">
         <v>4211583</v>
       </c>
-      <c r="G3" s="1">
-        <v>1342671</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1761321</v>
-      </c>
-      <c r="I3">
-        <v>697.76551700000005</v>
-      </c>
-      <c r="J3" s="1">
-        <v>20657.86</v>
-      </c>
-      <c r="K3" s="1">
-        <v>5886335</v>
-      </c>
-      <c r="L3" s="1">
-        <v>71236.19</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1157586</v>
-      </c>
-      <c r="N3">
-        <v>361.07586199999997</v>
-      </c>
-      <c r="O3" s="1">
-        <v>589469.30000000005</v>
-      </c>
-      <c r="P3">
-        <v>24.455172000000001</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>19556.43</v>
-      </c>
-      <c r="R3" s="1">
-        <v>-385401.9</v>
-      </c>
-      <c r="S3" s="1">
-        <v>669268</v>
-      </c>
-      <c r="T3">
-        <v>38.489654999999999</v>
-      </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
@@ -1309,48 +1183,7 @@
       <c r="F4" s="1">
         <v>26158430</v>
       </c>
-      <c r="G4" s="1">
-        <v>8121319</v>
-      </c>
-      <c r="H4" s="1">
-        <v>10936760</v>
-      </c>
-      <c r="I4">
-        <v>1075.1281260000001</v>
-      </c>
-      <c r="J4" s="1">
-        <v>1444650</v>
-      </c>
-      <c r="K4" s="1">
-        <v>36369160</v>
-      </c>
-      <c r="L4" s="1">
-        <v>434175.9</v>
-      </c>
-      <c r="M4" s="1">
-        <v>9682311</v>
-      </c>
-      <c r="N4">
-        <v>1445.9446840000001</v>
-      </c>
-      <c r="O4" s="1">
-        <v>3694784</v>
-      </c>
-      <c r="P4">
-        <v>79.527073000000001</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>119455.9</v>
-      </c>
-      <c r="R4" s="1">
-        <v>2386279</v>
-      </c>
-      <c r="S4" s="1">
-        <v>4059716</v>
-      </c>
-      <c r="T4">
-        <v>74.088358999999997</v>
-      </c>
+      <c r="I4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
@@ -1374,48 +1207,6 @@
       <c r="F5" s="1">
         <v>0</v>
       </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>-2604490</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>-7576788</v>
-      </c>
-      <c r="K5" s="1">
-        <v>-44093</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>0</v>
-      </c>
-      <c r="R5" s="1">
-        <v>-27992890</v>
-      </c>
-      <c r="S5" s="1">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1439,48 +1230,6 @@
       <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>32460</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
-        <v>252055</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1">
-        <v>-38346</v>
-      </c>
-      <c r="S6" s="1">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1504,48 +1253,6 @@
       <c r="F7" s="1">
         <v>608750</v>
       </c>
-      <c r="G7" s="1">
-        <v>300000</v>
-      </c>
-      <c r="H7" s="1">
-        <v>360528</v>
-      </c>
-      <c r="I7">
-        <v>114</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
-        <v>976037</v>
-      </c>
-      <c r="L7" s="1">
-        <v>21530</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>17</v>
-      </c>
-      <c r="O7" s="1">
-        <v>972</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0</v>
-      </c>
-      <c r="R7" s="1">
-        <v>0</v>
-      </c>
-      <c r="S7" s="1">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>4</v>
-      </c>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -1569,48 +1276,6 @@
       <c r="F8" s="1">
         <v>1729541</v>
       </c>
-      <c r="G8" s="1">
-        <v>800000</v>
-      </c>
-      <c r="H8" s="1">
-        <v>853064</v>
-      </c>
-      <c r="I8">
-        <v>900</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>2332399</v>
-      </c>
-      <c r="L8" s="1">
-        <v>53947</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>52</v>
-      </c>
-      <c r="O8" s="1">
-        <v>150656</v>
-      </c>
-      <c r="P8">
-        <v>14</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>0</v>
-      </c>
-      <c r="R8" s="1">
-        <v>0</v>
-      </c>
-      <c r="S8" s="1">
-        <v>375304</v>
-      </c>
-      <c r="T8">
-        <v>41</v>
-      </c>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
@@ -1634,51 +1299,513 @@
       <c r="F9" s="1">
         <v>311764000</v>
       </c>
-      <c r="G9" s="1">
-        <v>97343620</v>
-      </c>
-      <c r="H9" s="1">
-        <v>130322300</v>
-      </c>
-      <c r="I9">
-        <v>5521</v>
-      </c>
-      <c r="J9" s="1">
-        <v>15456290</v>
-      </c>
-      <c r="K9" s="1">
-        <v>434509500</v>
-      </c>
-      <c r="L9" s="1">
-        <v>5235198</v>
-      </c>
-      <c r="M9" s="1">
-        <v>83925000</v>
-      </c>
-      <c r="N9">
-        <v>14368</v>
-      </c>
-      <c r="O9" s="1">
-        <v>42667590</v>
-      </c>
-      <c r="P9">
-        <v>609</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>1398517</v>
-      </c>
-      <c r="R9" s="1">
-        <v>0</v>
-      </c>
-      <c r="S9" s="1">
-        <v>48521930</v>
-      </c>
-      <c r="T9">
-        <v>528</v>
-      </c>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>145</v>
+      </c>
+      <c r="C12" s="1">
+        <v>145</v>
+      </c>
+      <c r="D12">
+        <v>145</v>
+      </c>
+      <c r="E12" s="1">
+        <v>145</v>
+      </c>
+      <c r="F12" s="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1342671</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1761321</v>
+      </c>
+      <c r="D13">
+        <v>697.76551700000005</v>
+      </c>
+      <c r="E13" s="1">
+        <v>20657.86</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5886335</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8121319</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10936760</v>
+      </c>
+      <c r="D14">
+        <v>1075.1281260000001</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1444650</v>
+      </c>
+      <c r="F14" s="1">
+        <v>36369160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-2604490</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-7576788</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-44093</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>32460</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>252055</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>300000</v>
+      </c>
+      <c r="C17" s="1">
+        <v>360528</v>
+      </c>
+      <c r="D17">
+        <v>114</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>976037</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="B18" s="1">
+        <v>800000</v>
+      </c>
+      <c r="C18" s="1">
+        <v>853064</v>
+      </c>
+      <c r="D18">
+        <v>900</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2332399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>97343620</v>
+      </c>
+      <c r="C19" s="1">
+        <v>130322300</v>
+      </c>
+      <c r="D19">
+        <v>5521</v>
+      </c>
+      <c r="E19" s="1">
+        <v>15456290</v>
+      </c>
+      <c r="F19" s="1">
+        <v>434509500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1">
+        <v>145</v>
+      </c>
+      <c r="C22" s="1">
+        <v>145</v>
+      </c>
+      <c r="D22">
+        <v>145</v>
+      </c>
+      <c r="E22" s="1">
+        <v>145</v>
+      </c>
+      <c r="F22">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1">
+        <v>71236.19</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1157586</v>
+      </c>
+      <c r="D23">
+        <v>361.07586199999997</v>
+      </c>
+      <c r="E23" s="1">
+        <v>589469.30000000005</v>
+      </c>
+      <c r="F23">
+        <v>24.455172000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>434175.9</v>
+      </c>
+      <c r="C24" s="1">
+        <v>9682311</v>
+      </c>
+      <c r="D24">
+        <v>1445.9446840000001</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3694784</v>
+      </c>
+      <c r="F24">
+        <v>79.527073000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B27" s="1">
+        <v>21530</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>17</v>
+      </c>
+      <c r="E27" s="1">
+        <v>972</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="B28" s="1">
+        <v>53947</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>52</v>
+      </c>
+      <c r="E28" s="1">
+        <v>150656</v>
+      </c>
+      <c r="F28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1">
+        <v>5235198</v>
+      </c>
+      <c r="C29" s="1">
+        <v>83925000</v>
+      </c>
+      <c r="D29">
+        <v>14368</v>
+      </c>
+      <c r="E29" s="1">
+        <v>42667590</v>
+      </c>
+      <c r="F29">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1">
+        <v>145</v>
+      </c>
+      <c r="C32" s="1">
+        <v>145</v>
+      </c>
+      <c r="D32" s="1">
+        <v>145</v>
+      </c>
+      <c r="E32">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1">
+        <v>19556.43</v>
+      </c>
+      <c r="C33" s="1">
+        <v>-385401.9</v>
+      </c>
+      <c r="D33" s="1">
+        <v>669268</v>
+      </c>
+      <c r="E33">
+        <v>38.489654999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1">
+        <v>119455.9</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2386279</v>
+      </c>
+      <c r="D34" s="1">
+        <v>4059716</v>
+      </c>
+      <c r="E34">
+        <v>74.088358999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>-27992890</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>-38346</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
+        <v>375304</v>
+      </c>
+      <c r="E38">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1398517</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>48521930</v>
+      </c>
+      <c r="E39">
+        <v>528</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Project 5 version 2 after review.
</commit_message>
<xml_diff>
--- a/5_IdentifyFraudFromEnronEmail/final_project/data_description.xlsx
+++ b/5_IdentifyFraudFromEnronEmail/final_project/data_description.xlsx
@@ -9,17 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="10200" windowHeight="4665" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10200" windowHeight="4665" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1-copy" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="16_param" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$7:$M$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$7:$M$16</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
   <si>
     <t>count</t>
   </si>
@@ -193,6 +196,86 @@
   </si>
   <si>
     <t>Average precision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'split4_test_score': array(</t>
+  </si>
+  <si>
+    <t>'split2_train_score': array(</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'split4_train_score': array(</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'split2_test_score': array(</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'split3_train_score': array(</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'split0_train_score': array(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'split1_train_score': array(</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'split0_test_score': array(</t>
+  </si>
+  <si>
+    <t>'split3_test_score': array(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'split1_test_score': array(</t>
+  </si>
+  <si>
+    <t>'split4_test_score':</t>
+  </si>
+  <si>
+    <t>'split2_train_score':</t>
+  </si>
+  <si>
+    <t>'split4_train_score':</t>
+  </si>
+  <si>
+    <t>'split2_test_score':</t>
+  </si>
+  <si>
+    <t>'split3_train_score':</t>
+  </si>
+  <si>
+    <t>'split0_train_score':</t>
+  </si>
+  <si>
+    <t>'split1_train_score':</t>
+  </si>
+  <si>
+    <t>'split0_test_score':</t>
+  </si>
+  <si>
+    <t>'split3_test_score':</t>
+  </si>
+  <si>
+    <t>'split1_test_score':</t>
+  </si>
+  <si>
+    <t>F1  score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>split1_test_score':</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -200,7 +283,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +316,19 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -256,7 +352,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -277,6 +373,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1181,759 +1283,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W39"/>
-  <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>145</v>
-      </c>
-      <c r="C2" s="1">
-        <v>145</v>
-      </c>
-      <c r="D2" s="1">
-        <v>145</v>
-      </c>
-      <c r="E2" s="1">
-        <v>145</v>
-      </c>
-      <c r="F2" s="1">
-        <v>145</v>
-      </c>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>368334.2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1230.0137930000001</v>
-      </c>
-      <c r="D3" s="1">
-        <v>441822.7</v>
-      </c>
-      <c r="E3" s="1">
-        <v>4380626</v>
-      </c>
-      <c r="F3" s="1">
-        <v>4211583</v>
-      </c>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2211001</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2232.1530029999999</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2750583</v>
-      </c>
-      <c r="E4" s="1">
-        <v>27025390</v>
-      </c>
-      <c r="F4" s="1">
-        <v>26158430</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-102500</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>102500</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>210692</v>
-      </c>
-      <c r="C7" s="1">
-        <v>312</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>966522</v>
-      </c>
-      <c r="F7" s="1">
-        <v>608750</v>
-      </c>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="B8" s="1">
-        <v>271442</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1607</v>
-      </c>
-      <c r="D8" s="1">
-        <v>10259</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1979596</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1729541</v>
-      </c>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1">
-        <v>26704230</v>
-      </c>
-      <c r="C9" s="1">
-        <v>15149</v>
-      </c>
-      <c r="D9" s="1">
-        <v>32083400</v>
-      </c>
-      <c r="E9" s="1">
-        <v>309886600</v>
-      </c>
-      <c r="F9" s="1">
-        <v>311764000</v>
-      </c>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1">
-        <v>145</v>
-      </c>
-      <c r="C12" s="1">
-        <v>145</v>
-      </c>
-      <c r="D12">
-        <v>145</v>
-      </c>
-      <c r="E12" s="1">
-        <v>145</v>
-      </c>
-      <c r="F12" s="1">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1342671</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1761321</v>
-      </c>
-      <c r="D13">
-        <v>697.76551700000005</v>
-      </c>
-      <c r="E13" s="1">
-        <v>20657.86</v>
-      </c>
-      <c r="F13" s="1">
-        <v>5886335</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1">
-        <v>8121319</v>
-      </c>
-      <c r="C14" s="1">
-        <v>10936760</v>
-      </c>
-      <c r="D14">
-        <v>1075.1281260000001</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1444650</v>
-      </c>
-      <c r="F14" s="1">
-        <v>36369160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>-2604490</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>-7576788</v>
-      </c>
-      <c r="F15" s="1">
-        <v>-44093</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>32460</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>252055</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B17" s="1">
-        <v>300000</v>
-      </c>
-      <c r="C17" s="1">
-        <v>360528</v>
-      </c>
-      <c r="D17">
-        <v>114</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>976037</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="B18" s="1">
-        <v>800000</v>
-      </c>
-      <c r="C18" s="1">
-        <v>853064</v>
-      </c>
-      <c r="D18">
-        <v>900</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2332399</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1">
-        <v>97343620</v>
-      </c>
-      <c r="C19" s="1">
-        <v>130322300</v>
-      </c>
-      <c r="D19">
-        <v>5521</v>
-      </c>
-      <c r="E19" s="1">
-        <v>15456290</v>
-      </c>
-      <c r="F19" s="1">
-        <v>434509500</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="1">
-        <v>145</v>
-      </c>
-      <c r="C22" s="1">
-        <v>145</v>
-      </c>
-      <c r="D22">
-        <v>145</v>
-      </c>
-      <c r="E22" s="1">
-        <v>145</v>
-      </c>
-      <c r="F22">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="1">
-        <v>71236.19</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1157586</v>
-      </c>
-      <c r="D23">
-        <v>361.07586199999997</v>
-      </c>
-      <c r="E23" s="1">
-        <v>589469.30000000005</v>
-      </c>
-      <c r="F23">
-        <v>24.455172000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="1">
-        <v>434175.9</v>
-      </c>
-      <c r="C24" s="1">
-        <v>9682311</v>
-      </c>
-      <c r="D24">
-        <v>1445.9446840000001</v>
-      </c>
-      <c r="E24" s="1">
-        <v>3694784</v>
-      </c>
-      <c r="F24">
-        <v>79.527073000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="B26" s="1">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B27" s="1">
-        <v>21530</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>17</v>
-      </c>
-      <c r="E27" s="1">
-        <v>972</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="B28" s="1">
-        <v>53947</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>52</v>
-      </c>
-      <c r="E28" s="1">
-        <v>150656</v>
-      </c>
-      <c r="F28">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="1">
-        <v>5235198</v>
-      </c>
-      <c r="C29" s="1">
-        <v>83925000</v>
-      </c>
-      <c r="D29">
-        <v>14368</v>
-      </c>
-      <c r="E29" s="1">
-        <v>42667590</v>
-      </c>
-      <c r="F29">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1">
-        <v>145</v>
-      </c>
-      <c r="C32" s="1">
-        <v>145</v>
-      </c>
-      <c r="D32" s="1">
-        <v>145</v>
-      </c>
-      <c r="E32">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="1">
-        <v>19556.43</v>
-      </c>
-      <c r="C33" s="1">
-        <v>-385401.9</v>
-      </c>
-      <c r="D33" s="1">
-        <v>669268</v>
-      </c>
-      <c r="E33">
-        <v>38.489654999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="1">
-        <v>119455.9</v>
-      </c>
-      <c r="C34" s="1">
-        <v>2386279</v>
-      </c>
-      <c r="D34" s="1">
-        <v>4059716</v>
-      </c>
-      <c r="E34">
-        <v>74.088358999999997</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="1">
-        <v>0</v>
-      </c>
-      <c r="C35" s="1">
-        <v>-27992890</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="B36" s="1">
-        <v>0</v>
-      </c>
-      <c r="C36" s="1">
-        <v>-38346</v>
-      </c>
-      <c r="D36" s="1">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B37" s="1">
-        <v>0</v>
-      </c>
-      <c r="C37" s="1">
-        <v>0</v>
-      </c>
-      <c r="D37" s="1">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="B38" s="1">
-        <v>0</v>
-      </c>
-      <c r="C38" s="1">
-        <v>0</v>
-      </c>
-      <c r="D38" s="1">
-        <v>375304</v>
-      </c>
-      <c r="E38">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="1">
-        <v>1398517</v>
-      </c>
-      <c r="C39" s="1">
-        <v>0</v>
-      </c>
-      <c r="D39" s="1">
-        <v>48521930</v>
-      </c>
-      <c r="E39">
-        <v>528</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -2086,51 +1438,51 @@
         <v>49</v>
       </c>
       <c r="B4">
-        <f>AVERAGE(B7:B16)</f>
+        <f t="shared" ref="B4:M4" si="0">AVERAGE(B7:B16)</f>
         <v>0.139329805</v>
       </c>
       <c r="C4">
-        <f>AVERAGE(C7:C16)</f>
+        <f t="shared" si="0"/>
         <v>0.139329805</v>
       </c>
       <c r="D4">
-        <f>AVERAGE(D7:D16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f>AVERAGE(E7:E16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f>AVERAGE(F7:F16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f>AVERAGE(G7:G16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f>AVERAGE(H7:H16)</f>
+        <f t="shared" si="0"/>
         <v>0.28948439500000001</v>
       </c>
       <c r="I4">
-        <f>AVERAGE(I7:I16)</f>
+        <f t="shared" si="0"/>
         <v>0.139499558</v>
       </c>
       <c r="J4">
-        <f>AVERAGE(J7:J16)</f>
+        <f t="shared" si="0"/>
         <v>0.47261904700000007</v>
       </c>
       <c r="K4">
-        <f>AVERAGE(K7:K16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>AVERAGE(L7:L16)</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="M4">
-        <f>AVERAGE(M7:M16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2139,51 +1491,51 @@
         <v>47</v>
       </c>
       <c r="B5">
-        <f>AVERAGE(B18:B27)</f>
+        <f t="shared" ref="B5:M5" si="1">AVERAGE(B18:B27)</f>
         <v>1</v>
       </c>
       <c r="C5">
-        <f>AVERAGE(C18:C27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D5">
-        <f>AVERAGE(D18:D27)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>AVERAGE(E18:E27)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F5">
-        <f>AVERAGE(F18:F27)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G5">
-        <f>AVERAGE(G18:G27)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H5">
-        <f>AVERAGE(H18:H27)</f>
+        <f t="shared" si="1"/>
         <v>0.80909090999999989</v>
       </c>
       <c r="I5">
-        <f>AVERAGE(I18:I27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J5">
-        <f>AVERAGE(J18:J27)</f>
+        <f t="shared" si="1"/>
         <v>0.21454545399999997</v>
       </c>
       <c r="K5">
-        <f>AVERAGE(K18:K27)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L5">
-        <f>AVERAGE(L18:L27)</f>
+        <f t="shared" si="1"/>
         <v>3.6363635999999998E-2</v>
       </c>
       <c r="M5">
-        <f>AVERAGE(M18:M27)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3014,7 +2366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -3258,7 +2610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -3618,4 +2970,2030 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="A1:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="C2">
+        <v>0.1</v>
+      </c>
+      <c r="D2">
+        <v>0.11410488000000001</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>2*D2*E2/(D2+E2)</f>
+        <v>0.20483687316763213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>0.11410488000000001</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F17" si="0">2*D3*E3/(D3+E3)</f>
+        <v>0.20483687316763213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>100</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.1</v>
+      </c>
+      <c r="D10">
+        <v>0.33063927299999996</v>
+      </c>
+      <c r="E10">
+        <v>0.95</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.49054767563730645</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>100</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="C11">
+        <v>0.1</v>
+      </c>
+      <c r="D11">
+        <v>0.162938693</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.28021888682656459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>100</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D12">
+        <v>0.43940124900000005</v>
+      </c>
+      <c r="E12">
+        <v>0.75833333400000003</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.55640476420631868</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>100</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D13">
+        <v>0.63547619</v>
+      </c>
+      <c r="E13">
+        <v>0.31666666500000001</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.4226973394117553</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>100</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D14">
+        <v>0.68166666700000011</v>
+      </c>
+      <c r="E14">
+        <v>0.37777777599999995</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.48613878553817214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>100</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D15">
+        <v>0.65</v>
+      </c>
+      <c r="E15">
+        <v>0.116666666</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.19782608599810966</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>100</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="D16">
+        <v>0.8</v>
+      </c>
+      <c r="E16">
+        <v>0.28055555400000004</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.4154241628191197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>100</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:Q21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1">
+        <v>0.11428571</v>
+      </c>
+      <c r="C1">
+        <v>0.11428571</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>0.44444444</v>
+      </c>
+      <c r="K1">
+        <v>0.11428571</v>
+      </c>
+      <c r="L1">
+        <v>0.6</v>
+      </c>
+      <c r="M1">
+        <v>0.5</v>
+      </c>
+      <c r="N1">
+        <v>0.66666667000000002</v>
+      </c>
+      <c r="O1">
+        <v>0</v>
+      </c>
+      <c r="P1">
+        <v>1</v>
+      </c>
+      <c r="Q1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3">
+        <v>0.11392405</v>
+      </c>
+      <c r="C3">
+        <v>0.11392405</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0.39130435000000002</v>
+      </c>
+      <c r="K3">
+        <v>0.11538461999999999</v>
+      </c>
+      <c r="L3">
+        <v>0.47368420999999999</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0.5</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5">
+        <v>0.11392405</v>
+      </c>
+      <c r="C5">
+        <v>0.11392405</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0.28125</v>
+      </c>
+      <c r="K5">
+        <v>0.11538461999999999</v>
+      </c>
+      <c r="L5">
+        <v>0.4</v>
+      </c>
+      <c r="M5">
+        <v>0.6</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7">
+        <v>0.11428571</v>
+      </c>
+      <c r="C7">
+        <v>0.11428571</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0.375</v>
+      </c>
+      <c r="K7">
+        <v>0.11428571</v>
+      </c>
+      <c r="L7">
+        <v>0.375</v>
+      </c>
+      <c r="M7">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="N7">
+        <v>0.25</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9">
+        <v>0.11392405</v>
+      </c>
+      <c r="C9">
+        <v>0.11392405</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="K9">
+        <v>0.27272727000000002</v>
+      </c>
+      <c r="L9">
+        <v>0.4375</v>
+      </c>
+      <c r="M9">
+        <v>0.6</v>
+      </c>
+      <c r="N9">
+        <v>0.66666667000000002</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11">
+        <v>0.11392405</v>
+      </c>
+      <c r="C11">
+        <v>0.11392405</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0.375</v>
+      </c>
+      <c r="K11">
+        <v>0.19148936</v>
+      </c>
+      <c r="L11">
+        <v>0.72727273000000003</v>
+      </c>
+      <c r="M11">
+        <v>0.57142857000000002</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13">
+        <v>0.11392405</v>
+      </c>
+      <c r="C13">
+        <v>0.11392405</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0.3</v>
+      </c>
+      <c r="K13">
+        <v>0.13235294</v>
+      </c>
+      <c r="L13">
+        <v>0.45</v>
+      </c>
+      <c r="M13">
+        <v>0.75</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <v>0.11428571</v>
+      </c>
+      <c r="C15">
+        <v>0.11428571</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0.27272727000000002</v>
+      </c>
+      <c r="K15">
+        <v>0.22222222</v>
+      </c>
+      <c r="L15">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17">
+        <v>0.11428571</v>
+      </c>
+      <c r="C17">
+        <v>0.11428571</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0.26666666999999999</v>
+      </c>
+      <c r="K17">
+        <v>0.22222222</v>
+      </c>
+      <c r="L17">
+        <v>0.22222222</v>
+      </c>
+      <c r="M17">
+        <v>0.5</v>
+      </c>
+      <c r="N17">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0.5</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19">
+        <v>0.11428571</v>
+      </c>
+      <c r="C19">
+        <v>0.11428571</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0.26666666999999999</v>
+      </c>
+      <c r="K19">
+        <v>0.12903226000000001</v>
+      </c>
+      <c r="L19">
+        <v>0.375</v>
+      </c>
+      <c r="M19">
+        <v>0.5</v>
+      </c>
+      <c r="N19">
+        <v>0.4</v>
+      </c>
+      <c r="O19">
+        <v>0.5</v>
+      </c>
+      <c r="P19">
+        <v>0.5</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:AJ2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>1</v>
+      </c>
+      <c r="L1">
+        <v>0.75</v>
+      </c>
+      <c r="M1">
+        <v>0.25</v>
+      </c>
+      <c r="N1">
+        <v>0.5</v>
+      </c>
+      <c r="O1">
+        <v>0</v>
+      </c>
+      <c r="P1">
+        <v>0.25</v>
+      </c>
+      <c r="Q1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0.95</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>0.75833333400000003</v>
+      </c>
+      <c r="AF2">
+        <v>0.31666666500000001</v>
+      </c>
+      <c r="AG2">
+        <v>0.37777777599999995</v>
+      </c>
+      <c r="AH2">
+        <v>0.116666666</v>
+      </c>
+      <c r="AI2">
+        <v>0.28055555400000004</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0.22222222</v>
+      </c>
+      <c r="N3">
+        <v>0.22222222</v>
+      </c>
+      <c r="O3">
+        <v>0.11111111</v>
+      </c>
+      <c r="P3">
+        <v>0.22222222</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0.66666667000000002</v>
+      </c>
+      <c r="M5">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="N5">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="O5">
+        <v>0.11111111</v>
+      </c>
+      <c r="P5">
+        <v>0.22222222</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0.75</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0.75</v>
+      </c>
+      <c r="M7">
+        <v>0.25</v>
+      </c>
+      <c r="N7">
+        <v>0.25</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0.77777777999999997</v>
+      </c>
+      <c r="M9">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="N9">
+        <v>0.44444444</v>
+      </c>
+      <c r="O9">
+        <v>0.22222222</v>
+      </c>
+      <c r="P9">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0.88888889000000004</v>
+      </c>
+      <c r="M11">
+        <v>0.44444444</v>
+      </c>
+      <c r="N11">
+        <v>0.44444444</v>
+      </c>
+      <c r="O11">
+        <v>0.11111111</v>
+      </c>
+      <c r="P11">
+        <v>0.44444444</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="N13">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="O13">
+        <v>0.11111111</v>
+      </c>
+      <c r="P13">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0.75</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0.5</v>
+      </c>
+      <c r="M15">
+        <v>0.25</v>
+      </c>
+      <c r="N15">
+        <v>0.25</v>
+      </c>
+      <c r="O15">
+        <v>0.25</v>
+      </c>
+      <c r="P15">
+        <v>0.25</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0.5</v>
+      </c>
+      <c r="M17">
+        <v>0.25</v>
+      </c>
+      <c r="N17">
+        <v>0.5</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0.25</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>0.75</v>
+      </c>
+      <c r="M19">
+        <v>0.5</v>
+      </c>
+      <c r="N19">
+        <v>0.5</v>
+      </c>
+      <c r="O19">
+        <v>0.25</v>
+      </c>
+      <c r="P19">
+        <v>0.5</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>AVERAGE(B1:B19)</f>
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:P20" si="0">AVERAGE(C1:C19)</f>
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>0.75833333400000003</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>0.31666666500000001</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>0.37777777599999995</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>0.116666666</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="0"/>
+        <v>0.28055555400000004</v>
+      </c>
+      <c r="Q20">
+        <f>AVERAGE(Q1:Q19)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1">
+        <v>0.5</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>0.75</v>
+      </c>
+      <c r="E1">
+        <v>0.25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1">
+        <v>0.66666667000000002</v>
+      </c>
+      <c r="I1">
+        <v>0.8</v>
+      </c>
+      <c r="J1">
+        <v>0.6</v>
+      </c>
+      <c r="K1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0.22222222</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0.69230769000000003</v>
+      </c>
+      <c r="J2">
+        <v>0.47368420999999999</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.66666667000000002</v>
+      </c>
+      <c r="E3">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.69230769000000003</v>
+      </c>
+      <c r="J3">
+        <v>0.4</v>
+      </c>
+      <c r="K3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>0.25</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>0.75</v>
+      </c>
+      <c r="E4">
+        <v>0.25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0.4</v>
+      </c>
+      <c r="J4">
+        <v>0.375</v>
+      </c>
+      <c r="K4">
+        <v>0.33333332999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.77777777999999997</v>
+      </c>
+      <c r="E5">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0.75</v>
+      </c>
+      <c r="J5">
+        <v>0.4375</v>
+      </c>
+      <c r="K5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0.88888889000000004</v>
+      </c>
+      <c r="E6">
+        <v>0.44444444</v>
+      </c>
+      <c r="G6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0.81818181999999995</v>
+      </c>
+      <c r="J6">
+        <v>0.72727273000000003</v>
+      </c>
+      <c r="K6">
+        <v>0.57142857000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="G7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0.6</v>
+      </c>
+      <c r="J7">
+        <v>0.45</v>
+      </c>
+      <c r="K7">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8">
+        <v>0.25</v>
+      </c>
+      <c r="C8">
+        <v>0.75</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>0.25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8">
+        <v>0.5</v>
+      </c>
+      <c r="I8">
+        <v>0.5</v>
+      </c>
+      <c r="J8">
+        <v>0.33333332999999998</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>0.25</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+      <c r="E9">
+        <v>0.25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9">
+        <v>0.25</v>
+      </c>
+      <c r="I9">
+        <v>0.4</v>
+      </c>
+      <c r="J9">
+        <v>0.22222222</v>
+      </c>
+      <c r="K9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10">
+        <v>0.25</v>
+      </c>
+      <c r="C10">
+        <v>0.75</v>
+      </c>
+      <c r="D10">
+        <v>0.75</v>
+      </c>
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+      <c r="I10">
+        <v>0.6</v>
+      </c>
+      <c r="J10">
+        <v>0.375</v>
+      </c>
+      <c r="K10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f>AVERAGE(B1:B10)</f>
+        <v>0.65</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:E11" si="0">AVERAGE(C1:C10)</f>
+        <v>0.9</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.75833333400000003</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.31666666500000001</v>
+      </c>
+      <c r="H11">
+        <f>AVERAGE(H1:H10)</f>
+        <v>0.79166666699999999</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11" si="1">AVERAGE(I1:I10)</f>
+        <v>0.62527971999999998</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ref="J11" si="2">AVERAGE(J1:J10)</f>
+        <v>0.43940124900000005</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11" si="3">AVERAGE(K1:K10)</f>
+        <v>0.63547619</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0.65</v>
+      </c>
+      <c r="D15">
+        <v>0.9</v>
+      </c>
+      <c r="E15">
+        <v>0.75833333400000003</v>
+      </c>
+      <c r="F15">
+        <v>0.31666666500000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>0.79166666699999999</v>
+      </c>
+      <c r="D16">
+        <v>0.62527971999999998</v>
+      </c>
+      <c r="E16">
+        <v>0.43940124900000005</v>
+      </c>
+      <c r="F16">
+        <v>0.63547619</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f>2*C15*C16/(C15+C16)</f>
+        <v>0.71387283250546285</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:F17" si="4">2*D15*D16/(D15+D16)</f>
+        <v>0.73789973159808364</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>0.55640476420631868</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>0.4226973394117553</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>